<commit_message>
starting from scratch again on features
</commit_message>
<xml_diff>
--- a/feature_data_dictionary.xlsx
+++ b/feature_data_dictionary.xlsx
@@ -9,15 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="prod_features" sheetId="1" r:id="rId1"/>
-    <sheet name="user_features" sheetId="2" r:id="rId2"/>
-    <sheet name="order_features" sheetId="3" r:id="rId3"/>
-    <sheet name="dept_aisle_features" sheetId="4" r:id="rId4"/>
-    <sheet name="timing_features" sheetId="5" r:id="rId5"/>
-    <sheet name="dimreduc_features" sheetId="6" r:id="rId6"/>
+    <sheet name="user_orderheader" sheetId="9" r:id="rId1"/>
+    <sheet name="user_orderdetail" sheetId="12" r:id="rId2"/>
+    <sheet name="DIVIDER" sheetId="11" r:id="rId3"/>
+    <sheet name="prod_features" sheetId="1" r:id="rId4"/>
+    <sheet name="user_features" sheetId="7" r:id="rId5"/>
+    <sheet name="order_features" sheetId="3" r:id="rId6"/>
+    <sheet name="dept_aisle_features" sheetId="4" r:id="rId7"/>
+    <sheet name="timing_features" sheetId="5" r:id="rId8"/>
+    <sheet name="dimreduc_features" sheetId="6" r:id="rId9"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>fieldname</t>
   </si>
@@ -101,14 +105,116 @@
   </si>
   <si>
     <t>total number of reorders OVER the total number of times this has shown up at all within an order</t>
+  </si>
+  <si>
+    <t>user_orders</t>
+  </si>
+  <si>
+    <t>total number of orders this user has made all-time (coming from "orders" order-header table which has all three, train, test, priors)</t>
+  </si>
+  <si>
+    <t>user_period</t>
+  </si>
+  <si>
+    <t>sum of all days_since_prior_order, giving us the total amount of days this user spans across all datasets</t>
+  </si>
+  <si>
+    <t>user_mean_days_since_prior</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">average days between purchases
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I really want to do more with this. I'm thinking we could find the standard deviation for each user's days between purchases. Let's then match that up with a user/product average days between purchase. Cross reference that with a "days since this user purchased this item" field</t>
+    </r>
+  </si>
+  <si>
+    <t>total number of products each user has ever purchased (non distinct)</t>
+  </si>
+  <si>
+    <t>for every order except the user's very first purchase (which by definition cannot contain any reordered products), this is the ratio of total products reordered to the total number of orders</t>
+  </si>
+  <si>
+    <t>total number of distinct products this user has ever purchased</t>
+  </si>
+  <si>
+    <t>total reordered products over the total number of products that show up in all orders except for the first order of "this user"</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>user_reorder_dist_prod_ratio</t>
+  </si>
+  <si>
+    <t>each user's distinct reordered products over the total number of distinct products in all of the user's orders except for the first order</t>
+  </si>
+  <si>
+    <t>each user's distinct reordered products over the total number of reordered products by that user</t>
+  </si>
+  <si>
+    <t>User Features: #Products purchased, #Orders made, frequency and recency of orders, #Aisle purchased from, #Department purchased from, frequency and recency of reorders, tenure, mean order size, etc.
+Product Features: #users, #orders, order frequency, reorder rate, recency, mean add_to_cart_order, etc.
+Aisle and Department Features: similar to product features
+user product interaction:#purchases, #reorders, #day since last purchase, #order since last purchase etc.
+User aisle and department interaction: similar to product interaction
+User time interaction: user preferred day of week, user preferred time of day, similar features for products and aisles</t>
+  </si>
+  <si>
+    <t>user_od_product_variety</t>
+  </si>
+  <si>
+    <t>user_od_total_products</t>
+  </si>
+  <si>
+    <t>user_od_reorder_ratio</t>
+  </si>
+  <si>
+    <t>user_od_distinct_products</t>
+  </si>
+  <si>
+    <t>distinct number of products ordered divided by total number of products ever ordered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">me </t>
+  </si>
+  <si>
+    <t>002_user_features.R</t>
+  </si>
+  <si>
+    <t>user_od_reorder_prod_ratio</t>
+  </si>
+  <si>
+    <t>user_perc_prod_dept</t>
+  </si>
+  <si>
+    <t>user_reorder_dist_to_all_dist_prods</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -124,7 +230,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -132,14 +238,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,10 +579,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="148.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="234.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="1"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +995,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="72" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -625,19 +1028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -651,7 +1042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -663,7 +1054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>